<commit_message>
Combine Digital Album Sales into one file
</commit_message>
<xml_diff>
--- a/Digital_Album_Sales.xlsx
+++ b/Digital_Album_Sales.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17560" yWindow="760" windowWidth="26980" windowHeight="23180"/>
+    <workbookView xWindow="14960" yWindow="440" windowWidth="26980" windowHeight="23180"/>
   </bookViews>
   <sheets>
     <sheet name="RS Digital Sales Template v1_23" sheetId="1" r:id="rId1"/>
@@ -1250,10 +1250,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1267,10 +1267,7 @@
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
     <col min="9" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" customWidth="1"/>
-    <col min="13" max="242" width="8.83203125" customWidth="1"/>
+    <col min="10" max="238" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1328,7 +1325,7 @@
         <v>11</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -1357,7 +1354,7 @@
         <v>76</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -1386,7 +1383,7 @@
         <v>77</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -1415,7 +1412,7 @@
         <v>78</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -1444,7 +1441,7 @@
         <v>79</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -1473,7 +1470,7 @@
         <v>80</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -1502,7 +1499,7 @@
         <v>81</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -1560,7 +1557,7 @@
         <v>83</v>
       </c>
       <c r="I10">
-        <v>7</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -1589,7 +1586,7 @@
         <v>84</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -1647,7 +1644,7 @@
         <v>86</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -1676,7 +1673,7 @@
         <v>87</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -1734,10 +1731,10 @@
         <v>89</v>
       </c>
       <c r="I16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1763,10 +1760,10 @@
         <v>90</v>
       </c>
       <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1792,10 +1789,10 @@
         <v>91</v>
       </c>
       <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1821,10 +1818,10 @@
         <v>92</v>
       </c>
       <c r="I19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1850,10 +1847,10 @@
         <v>93</v>
       </c>
       <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1879,10 +1876,10 @@
         <v>94</v>
       </c>
       <c r="I21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1908,10 +1905,10 @@
         <v>95</v>
       </c>
       <c r="I22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1937,10 +1934,10 @@
         <v>96</v>
       </c>
       <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1966,10 +1963,10 @@
         <v>97</v>
       </c>
       <c r="I24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1995,10 +1992,10 @@
         <v>98</v>
       </c>
       <c r="I25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -2024,10 +2021,10 @@
         <v>172</v>
       </c>
       <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2053,10 +2050,10 @@
         <v>99</v>
       </c>
       <c r="I27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2084,10 +2081,8 @@
       <c r="I28">
         <v>0</v>
       </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2115,10 +2110,8 @@
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2144,12 +2137,10 @@
         <v>102</v>
       </c>
       <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2175,12 +2166,10 @@
         <v>103</v>
       </c>
       <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-    </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2206,12 +2195,10 @@
         <v>104</v>
       </c>
       <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-    </row>
-    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -2237,12 +2224,10 @@
         <v>105</v>
       </c>
       <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-    </row>
-    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -2268,12 +2253,10 @@
         <v>106</v>
       </c>
       <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-    </row>
-    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2299,12 +2282,10 @@
         <v>107</v>
       </c>
       <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-    </row>
-    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2330,12 +2311,10 @@
         <v>108</v>
       </c>
       <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-    </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2361,12 +2340,10 @@
         <v>109</v>
       </c>
       <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-    </row>
-    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2392,12 +2369,10 @@
         <v>110</v>
       </c>
       <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-    </row>
-    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2423,12 +2398,10 @@
         <v>111</v>
       </c>
       <c r="I39">
-        <v>2</v>
-      </c>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-    </row>
-    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2454,12 +2427,10 @@
         <v>112</v>
       </c>
       <c r="I40">
-        <v>3</v>
-      </c>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-    </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2485,12 +2456,10 @@
         <v>113</v>
       </c>
       <c r="I41">
-        <v>2</v>
-      </c>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-    </row>
-    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2516,12 +2485,10 @@
         <v>114</v>
       </c>
       <c r="I42">
-        <v>3</v>
-      </c>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-    </row>
-    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2547,12 +2514,10 @@
         <v>173</v>
       </c>
       <c r="I43">
-        <v>8</v>
-      </c>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-    </row>
-    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2578,12 +2543,10 @@
         <v>115</v>
       </c>
       <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-    </row>
-    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2609,12 +2572,10 @@
         <v>116</v>
       </c>
       <c r="I45">
-        <v>1</v>
-      </c>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-    </row>
-    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2640,12 +2601,10 @@
         <v>117</v>
       </c>
       <c r="I46">
-        <v>7</v>
-      </c>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-    </row>
-    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2671,12 +2630,10 @@
         <v>118</v>
       </c>
       <c r="I47">
-        <v>3</v>
-      </c>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-    </row>
-    <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2702,12 +2659,10 @@
         <v>119</v>
       </c>
       <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-    </row>
-    <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2733,12 +2688,10 @@
         <v>120</v>
       </c>
       <c r="I49">
-        <v>2</v>
-      </c>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
-    </row>
-    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2764,12 +2717,10 @@
         <v>121</v>
       </c>
       <c r="I50">
-        <v>0</v>
-      </c>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-    </row>
-    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2795,12 +2746,10 @@
         <v>122</v>
       </c>
       <c r="I51">
-        <v>1</v>
-      </c>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-    </row>
-    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2826,12 +2775,10 @@
         <v>123</v>
       </c>
       <c r="I52">
-        <v>1</v>
-      </c>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-    </row>
-    <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2857,12 +2804,10 @@
         <v>124</v>
       </c>
       <c r="I53">
-        <v>0</v>
-      </c>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-    </row>
-    <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2888,12 +2833,10 @@
         <v>125</v>
       </c>
       <c r="I54">
-        <v>0</v>
-      </c>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-    </row>
-    <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2921,10 +2864,8 @@
       <c r="I55">
         <v>0</v>
       </c>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-    </row>
-    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2950,12 +2891,10 @@
         <v>127</v>
       </c>
       <c r="I56">
-        <v>1</v>
-      </c>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-    </row>
-    <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2983,10 +2922,8 @@
       <c r="I57">
         <v>1</v>
       </c>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-    </row>
-    <row r="58" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -3012,12 +2949,10 @@
         <v>129</v>
       </c>
       <c r="I58">
-        <v>0</v>
-      </c>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
-    </row>
-    <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -3045,10 +2980,8 @@
       <c r="I59">
         <v>0</v>
       </c>
-      <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
-    </row>
-    <row r="60" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -3074,12 +3007,10 @@
         <v>130</v>
       </c>
       <c r="I60">
-        <v>10</v>
-      </c>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
-    </row>
-    <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -3107,10 +3038,8 @@
       <c r="I61">
         <v>4</v>
       </c>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-    </row>
-    <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -3136,12 +3065,10 @@
         <v>139</v>
       </c>
       <c r="I62">
-        <v>7</v>
-      </c>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
-    </row>
-    <row r="63" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -3169,10 +3096,8 @@
       <c r="I63">
         <v>0</v>
       </c>
-      <c r="K63" s="6"/>
-      <c r="L63" s="6"/>
-    </row>
-    <row r="64" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -3198,12 +3123,10 @@
         <v>133</v>
       </c>
       <c r="I64">
-        <v>4</v>
-      </c>
-      <c r="K64" s="6"/>
-      <c r="L64" s="6"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -3229,10 +3152,10 @@
         <v>134</v>
       </c>
       <c r="I65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -3260,10 +3183,8 @@
       <c r="I66">
         <v>5</v>
       </c>
-      <c r="K66" s="6"/>
-      <c r="L66" s="6"/>
-    </row>
-    <row r="67" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -3289,12 +3210,10 @@
         <v>165</v>
       </c>
       <c r="I67">
-        <v>2</v>
-      </c>
-      <c r="K67" s="6"/>
-      <c r="L67" s="6"/>
-    </row>
-    <row r="68" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -3320,12 +3239,10 @@
         <v>136</v>
       </c>
       <c r="I68">
-        <v>0</v>
-      </c>
-      <c r="K68" s="6"/>
-      <c r="L68" s="6"/>
-    </row>
-    <row r="69" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -3351,12 +3268,10 @@
         <v>137</v>
       </c>
       <c r="I69">
-        <v>4</v>
-      </c>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-    </row>
-    <row r="70" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -3382,12 +3297,10 @@
         <v>166</v>
       </c>
       <c r="I70">
-        <v>4</v>
-      </c>
-      <c r="K70" s="6"/>
-      <c r="L70" s="6"/>
-    </row>
-    <row r="71" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -3415,10 +3328,8 @@
       <c r="I71">
         <v>5</v>
       </c>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-    </row>
-    <row r="72" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -3444,12 +3355,10 @@
         <v>138</v>
       </c>
       <c r="I72">
-        <v>0</v>
-      </c>
-      <c r="K72" s="6"/>
-      <c r="L72" s="6"/>
-    </row>
-    <row r="73" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -3475,10 +3384,8 @@
         <v>177</v>
       </c>
       <c r="I73">
-        <v>10</v>
-      </c>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.22" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Digital Album Sales File Processing
</commit_message>
<xml_diff>
--- a/Digital_Album_Sales.xlsx
+++ b/Digital_Album_Sales.xlsx
@@ -297,9 +297,6 @@
     <t>sale-month</t>
   </si>
   <si>
-    <t>upc-ean</t>
-  </si>
-  <si>
     <t>Basin Street Records</t>
   </si>
   <si>
@@ -821,6 +818,9 @@
   </si>
   <si>
     <t>net-units</t>
+  </si>
+  <si>
+    <t>upc</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1290,39 +1290,39 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>7</v>
+        <v>180</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2022</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>2022</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="4">
         <v>652905010129</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <v>24</v>
@@ -1330,28 +1330,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2022</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>2022</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="5">
         <v>652905010228</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I3">
         <v>11</v>
@@ -1359,28 +1359,28 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2022</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>2022</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="5">
         <v>652905010327</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I4">
         <v>31</v>
@@ -1388,28 +1388,28 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2022</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>2022</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5">
         <v>652905010426</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I5">
         <v>23</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>2022</v>
@@ -1426,19 +1426,19 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5">
         <v>652905010525</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6">
         <v>75</v>
@@ -1446,28 +1446,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>2022</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>2022</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="5">
         <v>652905010624</v>
       </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I7">
         <v>26</v>
@@ -1475,28 +1475,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2022</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>2022</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="5">
         <v>652905010723</v>
       </c>
       <c r="H8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8">
         <v>41</v>
@@ -1504,28 +1504,28 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2022</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>2022</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>179</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="5">
         <v>652905010822</v>
       </c>
       <c r="H9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -1533,28 +1533,28 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>2022</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>2022</v>
-      </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>179</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="5">
         <v>652905010921</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I10">
         <v>86</v>
@@ -1562,28 +1562,28 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>2022</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>2022</v>
-      </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>179</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="5">
         <v>652905011126</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I11">
         <v>18</v>
@@ -1591,28 +1591,28 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>2022</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" t="s">
         <v>8</v>
       </c>
-      <c r="B12">
-        <v>2022</v>
-      </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>179</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" s="5">
         <v>652905011225</v>
       </c>
       <c r="H12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1620,28 +1620,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>2022</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" t="s">
         <v>8</v>
       </c>
-      <c r="B13">
-        <v>2022</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="5">
         <v>652905011324</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -1649,28 +1649,28 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>2022</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="B14">
-        <v>2022</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>179</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" s="5">
         <v>652905011423</v>
       </c>
       <c r="H14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I14">
         <v>15</v>
@@ -1678,28 +1678,28 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>2022</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" t="s">
         <v>8</v>
       </c>
-      <c r="B15">
-        <v>2022</v>
-      </c>
-      <c r="C15">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>179</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="5">
         <v>652905011522</v>
       </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I15">
         <v>6</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>2022</v>
@@ -1716,19 +1716,19 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="5">
         <v>652905020128</v>
       </c>
       <c r="H16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I16">
         <v>8</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>2022</v>
@@ -1745,19 +1745,19 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="5">
         <v>652905020227</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I17">
         <v>8</v>
@@ -1765,7 +1765,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>2022</v>
@@ -1774,19 +1774,19 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="5">
         <v>652905020326</v>
       </c>
       <c r="H18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -1794,7 +1794,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>2022</v>
@@ -1803,19 +1803,19 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G19" s="5">
         <v>652905020425</v>
       </c>
       <c r="H19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I19">
         <v>13</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>2022</v>
@@ -1832,19 +1832,19 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" s="5">
         <v>652905020623</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I20">
         <v>5</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>2022</v>
@@ -1861,19 +1861,19 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21" s="5">
         <v>652905030127</v>
       </c>
       <c r="H21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I21">
         <v>3</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22">
         <v>2022</v>
@@ -1890,19 +1890,19 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G22" s="5">
         <v>652905030226</v>
       </c>
       <c r="H22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I22">
         <v>6</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23">
         <v>2022</v>
@@ -1919,19 +1919,19 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G23" s="5">
         <v>652905030325</v>
       </c>
       <c r="H23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I23">
         <v>9</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24">
         <v>2022</v>
@@ -1948,19 +1948,19 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G24" s="5">
         <v>652905030424</v>
       </c>
       <c r="H24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I24">
         <v>6</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>2022</v>
@@ -1977,19 +1977,19 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G25" s="5">
         <v>652905030523</v>
       </c>
       <c r="H25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I25">
         <v>6</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26">
         <v>2022</v>
@@ -2006,19 +2006,19 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G26" s="5">
         <v>652905030622</v>
       </c>
       <c r="H26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I26">
         <v>18</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27">
         <v>2022</v>
@@ -2035,19 +2035,19 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="5">
         <v>652905040126</v>
       </c>
       <c r="H27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I27">
         <v>3</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28">
         <v>2022</v>
@@ -2064,19 +2064,19 @@
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28" s="5">
         <v>652905040225</v>
       </c>
       <c r="H28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29">
         <v>2022</v>
@@ -2093,19 +2093,19 @@
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" s="5">
         <v>652905040324</v>
       </c>
       <c r="H29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2113,7 +2113,7 @@
     </row>
     <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30">
         <v>2022</v>
@@ -2122,19 +2122,19 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G30" s="5">
         <v>652905040423</v>
       </c>
       <c r="H30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I30">
         <v>4</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31">
         <v>2022</v>
@@ -2151,19 +2151,19 @@
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G31" s="5">
         <v>652905040522</v>
       </c>
       <c r="H31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I31">
         <v>37</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32">
         <v>2022</v>
@@ -2180,19 +2180,19 @@
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32" s="7">
         <v>652905040621</v>
       </c>
       <c r="H32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I32">
         <v>12</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33">
         <v>2022</v>
@@ -2209,19 +2209,19 @@
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G33" s="7">
         <v>652905040720</v>
       </c>
       <c r="H33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I33">
         <v>42</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34">
         <v>2022</v>
@@ -2238,19 +2238,19 @@
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G34" s="7">
         <v>652905040836</v>
       </c>
       <c r="H34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I34">
         <v>9</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35">
         <v>2022</v>
@@ -2267,19 +2267,19 @@
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G35" s="7">
         <v>652905040928</v>
       </c>
       <c r="H35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I35">
         <v>4</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36">
         <v>2022</v>
@@ -2296,19 +2296,19 @@
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G36" s="5">
         <v>652905050125</v>
       </c>
       <c r="H36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I36">
         <v>12</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37">
         <v>2022</v>
@@ -2325,19 +2325,19 @@
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G37" s="5">
         <v>652905050224</v>
       </c>
       <c r="H37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I37">
         <v>23</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38">
         <v>2022</v>
@@ -2354,19 +2354,19 @@
         <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G38" s="5">
         <v>652905050323</v>
       </c>
       <c r="H38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I38">
         <v>24</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39">
         <v>2022</v>
@@ -2383,19 +2383,19 @@
         <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G39" s="5">
         <v>652905050422</v>
       </c>
       <c r="H39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I39">
         <v>18</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40">
         <v>2022</v>
@@ -2412,19 +2412,19 @@
         <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G40" s="7">
         <v>652905050521</v>
       </c>
       <c r="H40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I40">
         <v>15</v>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41">
         <v>2022</v>
@@ -2441,19 +2441,19 @@
         <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G41" s="7">
         <v>652905050620</v>
       </c>
       <c r="H41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I41">
         <v>13</v>
@@ -2461,7 +2461,7 @@
     </row>
     <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42">
         <v>2022</v>
@@ -2470,19 +2470,19 @@
         <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G42" s="7">
         <v>652905050729</v>
       </c>
       <c r="H42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I42">
         <v>11</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43">
         <v>2022</v>
@@ -2499,19 +2499,19 @@
         <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G43" s="7">
         <v>652905050828</v>
       </c>
       <c r="H43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I43">
         <v>17</v>
@@ -2519,7 +2519,7 @@
     </row>
     <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44">
         <v>2022</v>
@@ -2528,19 +2528,19 @@
         <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G44" s="5">
         <v>652905060124</v>
       </c>
       <c r="H44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I44">
         <v>18</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45">
         <v>2022</v>
@@ -2557,19 +2557,19 @@
         <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G45" s="5">
         <v>652905071328</v>
       </c>
       <c r="H45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I45">
         <v>40</v>
@@ -2577,7 +2577,7 @@
     </row>
     <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46">
         <v>2022</v>
@@ -2586,19 +2586,19 @@
         <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G46" s="5">
         <v>652905071724</v>
       </c>
       <c r="H46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I46">
         <v>50</v>
@@ -2606,7 +2606,7 @@
     </row>
     <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47">
         <v>2022</v>
@@ -2615,19 +2615,19 @@
         <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G47" s="5">
         <v>652905071823</v>
       </c>
       <c r="H47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I47">
         <v>6</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B48">
         <v>2022</v>
@@ -2644,19 +2644,19 @@
         <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G48" s="5">
         <v>652905080122</v>
       </c>
       <c r="H48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I48">
         <v>2</v>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B49">
         <v>2022</v>
@@ -2673,19 +2673,19 @@
         <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G49" s="5">
         <v>652905080221</v>
       </c>
       <c r="H49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I49">
         <v>11</v>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B50">
         <v>2022</v>
@@ -2702,19 +2702,19 @@
         <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G50" s="5">
         <v>652905080320</v>
       </c>
       <c r="H50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I50">
         <v>18</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B51">
         <v>2022</v>
@@ -2731,19 +2731,19 @@
         <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G51" s="5">
         <v>652905090121</v>
       </c>
       <c r="H51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I51">
         <v>116</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B52">
         <v>2022</v>
@@ -2760,19 +2760,19 @@
         <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G52" s="5">
         <v>652905090220</v>
       </c>
       <c r="H52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I52">
         <v>50</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B53">
         <v>2022</v>
@@ -2789,19 +2789,19 @@
         <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G53" s="5">
         <v>652905100127</v>
       </c>
       <c r="H53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B54">
         <v>2022</v>
@@ -2818,19 +2818,19 @@
         <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G54" s="5">
         <v>652905100226</v>
       </c>
       <c r="H54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I54">
         <v>2</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B55">
         <v>2022</v>
@@ -2847,19 +2847,19 @@
         <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G55" s="5">
         <v>652905100325</v>
       </c>
       <c r="H55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B56">
         <v>2022</v>
@@ -2876,19 +2876,19 @@
         <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G56" s="5">
         <v>652905100424</v>
       </c>
       <c r="H56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I56">
         <v>12</v>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="57" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B57">
         <v>2022</v>
@@ -2905,19 +2905,19 @@
         <v>12</v>
       </c>
       <c r="D57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G57" s="7">
         <v>652905100523</v>
       </c>
       <c r="H57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -2925,7 +2925,7 @@
     </row>
     <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B58">
         <v>2022</v>
@@ -2934,19 +2934,19 @@
         <v>12</v>
       </c>
       <c r="D58" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G58" s="5">
         <v>652905110126</v>
       </c>
       <c r="H58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I58">
         <v>12</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B59">
         <v>2022</v>
@@ -2963,19 +2963,19 @@
         <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G59" s="5">
         <v>652905120125</v>
       </c>
       <c r="H59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B60">
         <v>2022</v>
@@ -2992,19 +2992,19 @@
         <v>12</v>
       </c>
       <c r="D60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G60" s="7">
         <v>652905120224</v>
       </c>
       <c r="H60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I60">
         <v>105</v>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B61">
         <v>2022</v>
@@ -3021,19 +3021,19 @@
         <v>12</v>
       </c>
       <c r="D61" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G61" s="7">
         <v>652905120323</v>
       </c>
       <c r="H61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I61">
         <v>4</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B62">
         <v>2022</v>
@@ -3050,19 +3050,19 @@
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G62" s="7">
         <v>652905120422</v>
       </c>
       <c r="H62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I62">
         <v>54</v>
@@ -3070,7 +3070,7 @@
     </row>
     <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B63">
         <v>2022</v>
@@ -3079,19 +3079,19 @@
         <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G63" s="7">
         <v>652905140123</v>
       </c>
       <c r="H63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B64">
         <v>2022</v>
@@ -3108,19 +3108,19 @@
         <v>12</v>
       </c>
       <c r="D64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G64" s="7">
         <v>652905140222</v>
       </c>
       <c r="H64" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I64">
         <v>10</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B65">
         <v>2022</v>
@@ -3137,19 +3137,19 @@
         <v>12</v>
       </c>
       <c r="D65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G65" s="5">
         <v>652905140420</v>
       </c>
       <c r="H65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I65">
         <v>13</v>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B66">
         <v>2022</v>
@@ -3166,19 +3166,19 @@
         <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G66" s="8">
         <v>652905140529</v>
       </c>
       <c r="H66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I66">
         <v>5</v>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B67">
         <v>2022</v>
@@ -3195,19 +3195,19 @@
         <v>12</v>
       </c>
       <c r="D67" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G67" s="8">
         <v>652905140628</v>
       </c>
       <c r="H67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I67">
         <v>9</v>
@@ -3215,7 +3215,7 @@
     </row>
     <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B68">
         <v>2022</v>
@@ -3224,19 +3224,19 @@
         <v>12</v>
       </c>
       <c r="D68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G68" s="5">
         <v>652905150122</v>
       </c>
       <c r="H68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I68">
         <v>1</v>
@@ -3244,7 +3244,7 @@
     </row>
     <row r="69" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B69">
         <v>2022</v>
@@ -3253,19 +3253,19 @@
         <v>12</v>
       </c>
       <c r="D69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G69" s="5">
         <v>652905160121</v>
       </c>
       <c r="H69" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I69">
         <v>30</v>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B70">
         <v>2022</v>
@@ -3282,19 +3282,19 @@
         <v>12</v>
       </c>
       <c r="D70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G70" s="5">
         <v>652905160220</v>
       </c>
       <c r="H70" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I70">
         <v>48</v>
@@ -3302,7 +3302,7 @@
     </row>
     <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B71">
         <v>2022</v>
@@ -3311,19 +3311,19 @@
         <v>12</v>
       </c>
       <c r="D71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G71" s="5">
         <v>652905160428</v>
       </c>
       <c r="H71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I71">
         <v>5</v>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B72">
         <v>2022</v>
@@ -3340,19 +3340,19 @@
         <v>12</v>
       </c>
       <c r="D72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G72" s="5">
         <v>652905170120</v>
       </c>
       <c r="H72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I72">
         <v>6</v>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B73">
         <v>2022</v>
@@ -3369,19 +3369,19 @@
         <v>12</v>
       </c>
       <c r="D73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G73" s="5">
         <v>652905180129</v>
       </c>
       <c r="H73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I73">
         <v>78</v>

</xml_diff>

<commit_message>
Fix Digital Album Sales to correctly match previous royalty runs
</commit_message>
<xml_diff>
--- a/Digital_Album_Sales.xlsx
+++ b/Digital_Album_Sales.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14960" yWindow="440" windowWidth="26980" windowHeight="23180"/>
+    <workbookView xWindow="1480" yWindow="2480" windowWidth="26980" windowHeight="23180"/>
   </bookViews>
   <sheets>
     <sheet name="RS Digital Sales Template v1_23" sheetId="1" r:id="rId1"/>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1267,7 +1267,7 @@
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
     <col min="9" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="238" width="8.83203125" customWidth="1"/>
+    <col min="10" max="233" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1325,7 +1325,7 @@
         <v>11</v>
       </c>
       <c r="I2">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -1354,7 +1354,7 @@
         <v>76</v>
       </c>
       <c r="I3">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -1383,7 +1383,7 @@
         <v>77</v>
       </c>
       <c r="I4">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -1412,7 +1412,7 @@
         <v>78</v>
       </c>
       <c r="I5">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -1441,7 +1441,7 @@
         <v>79</v>
       </c>
       <c r="I6">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -1470,7 +1470,7 @@
         <v>80</v>
       </c>
       <c r="I7">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -1499,7 +1499,7 @@
         <v>81</v>
       </c>
       <c r="I8">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -1557,7 +1557,7 @@
         <v>83</v>
       </c>
       <c r="I10">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -1586,7 +1586,7 @@
         <v>84</v>
       </c>
       <c r="I11">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -1673,7 +1673,7 @@
         <v>87</v>
       </c>
       <c r="I14">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -1731,7 +1731,7 @@
         <v>89</v>
       </c>
       <c r="I16">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
@@ -1760,7 +1760,7 @@
         <v>90</v>
       </c>
       <c r="I17">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
@@ -1789,7 +1789,7 @@
         <v>91</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
@@ -1818,7 +1818,7 @@
         <v>92</v>
       </c>
       <c r="I19">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
@@ -1847,7 +1847,7 @@
         <v>93</v>
       </c>
       <c r="I20">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
@@ -1876,7 +1876,7 @@
         <v>94</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
@@ -1905,7 +1905,7 @@
         <v>95</v>
       </c>
       <c r="I22">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
@@ -1934,7 +1934,7 @@
         <v>96</v>
       </c>
       <c r="I23">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
@@ -1963,7 +1963,7 @@
         <v>97</v>
       </c>
       <c r="I24">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
@@ -1992,7 +1992,7 @@
         <v>98</v>
       </c>
       <c r="I25">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
@@ -2021,7 +2021,7 @@
         <v>172</v>
       </c>
       <c r="I26">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
@@ -2166,7 +2166,7 @@
         <v>103</v>
       </c>
       <c r="I31">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2195,7 +2195,7 @@
         <v>104</v>
       </c>
       <c r="I32">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2224,7 +2224,7 @@
         <v>105</v>
       </c>
       <c r="I33">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2253,7 +2253,7 @@
         <v>106</v>
       </c>
       <c r="I34">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2282,7 +2282,7 @@
         <v>107</v>
       </c>
       <c r="I35">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2311,7 +2311,7 @@
         <v>108</v>
       </c>
       <c r="I36">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2340,7 +2340,7 @@
         <v>109</v>
       </c>
       <c r="I37">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2369,7 +2369,7 @@
         <v>110</v>
       </c>
       <c r="I38">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2398,7 +2398,7 @@
         <v>111</v>
       </c>
       <c r="I39">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2427,7 +2427,7 @@
         <v>112</v>
       </c>
       <c r="I40">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2456,7 +2456,7 @@
         <v>113</v>
       </c>
       <c r="I41">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2485,7 +2485,7 @@
         <v>114</v>
       </c>
       <c r="I42">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2514,7 +2514,7 @@
         <v>173</v>
       </c>
       <c r="I43">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2543,7 +2543,7 @@
         <v>115</v>
       </c>
       <c r="I44">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2572,7 +2572,7 @@
         <v>116</v>
       </c>
       <c r="I45">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2601,7 +2601,7 @@
         <v>117</v>
       </c>
       <c r="I46">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2688,7 +2688,7 @@
         <v>120</v>
       </c>
       <c r="I49">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2717,7 +2717,7 @@
         <v>121</v>
       </c>
       <c r="I50">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2746,7 +2746,7 @@
         <v>122</v>
       </c>
       <c r="I51">
-        <v>116</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2775,7 +2775,7 @@
         <v>123</v>
       </c>
       <c r="I52">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2833,7 +2833,7 @@
         <v>125</v>
       </c>
       <c r="I54">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2891,7 +2891,7 @@
         <v>127</v>
       </c>
       <c r="I56">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -2949,7 +2949,7 @@
         <v>129</v>
       </c>
       <c r="I58">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -3007,7 +3007,7 @@
         <v>130</v>
       </c>
       <c r="I60">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -3065,7 +3065,7 @@
         <v>139</v>
       </c>
       <c r="I62">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -3123,7 +3123,7 @@
         <v>133</v>
       </c>
       <c r="I64">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.15">
@@ -3152,7 +3152,7 @@
         <v>134</v>
       </c>
       <c r="I65">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -3210,7 +3210,7 @@
         <v>165</v>
       </c>
       <c r="I67">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -3268,7 +3268,7 @@
         <v>137</v>
       </c>
       <c r="I69">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -3297,7 +3297,7 @@
         <v>166</v>
       </c>
       <c r="I70">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -3355,7 +3355,7 @@
         <v>138</v>
       </c>
       <c r="I72">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -3384,7 +3384,7 @@
         <v>177</v>
       </c>
       <c r="I73">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>